<commit_message>
Now a functioning but slow performing model
</commit_message>
<xml_diff>
--- a/test/Sample data/GUCHamb_Timeslot_test.xlsx
+++ b/test/Sample data/GUCHamb_Timeslot_test.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="23">
   <si>
     <t>Timeslot</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>AEKG</t>
+  </si>
+  <si>
+    <t>Holter</t>
   </si>
 </sst>
 </file>
@@ -950,7 +953,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1930,157 +1933,401 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0.39583333333333331</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="M24" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="N24" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="O24" s="1">
+        <v>0.41666666666666669</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="O25" s="1">
+        <v>0.4375</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="O26" s="1">
+        <v>0.46875</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="M27" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="O27" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L28" t="s">
+        <v>12</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N28" t="s">
+        <v>12</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="N29" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="O29" s="1">
+        <v>0.57291666666666663</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="L30" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="M30" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="N30" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="O30" s="1">
+        <v>0.60416666666666663</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
+      <c r="A31" s="4">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
+      <c r="F31" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="I31" s="5">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="J31" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="K31" s="5">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="L31" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="M31" s="5">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="N31" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="O31" s="5">
+        <v>0.63541666666666663</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
@@ -2158,12 +2405,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2299,15 +2543,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD84CE38-E42E-4165-94C0-E9F0263CCA00}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85C72108-22AD-4B4C-AD2F-243F6F7C20B2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6edaa03f-8cd3-4dde-a2dc-6fcdfb7e57e2"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2331,17 +2586,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85C72108-22AD-4B4C-AD2F-243F6F7C20B2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD84CE38-E42E-4165-94C0-E9F0263CCA00}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="6edaa03f-8cd3-4dde-a2dc-6fcdfb7e57e2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Restructuring, not done just backing up the work
</commit_message>
<xml_diff>
--- a/test/Sample data/GUCHamb_Timeslot_test.xlsx
+++ b/test/Sample data/GUCHamb_Timeslot_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12822" windowHeight="6424" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12822" windowHeight="6424"/>
   </bookViews>
   <sheets>
     <sheet name="GUCH AMB" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="29">
   <si>
     <t>Timeslot</t>
   </si>
@@ -94,6 +94,24 @@
   </si>
   <si>
     <t>Holter</t>
+  </si>
+  <si>
+    <t>MRS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Even</t>
+  </si>
+  <si>
+    <t>Acute</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>Odd</t>
   </si>
 </sst>
 </file>
@@ -427,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -736,212 +754,970 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+    <row r="10" spans="1:15" s="4" customFormat="1" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="G10" s="5">
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G10" s="3">
         <v>0.63541666666666663</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
     </row>
     <row r="11" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11"/>
+      <c r="F11" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14"/>
+      <c r="F14" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
     </row>
     <row r="16" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="G16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="O16" s="5"/>
-    </row>
-    <row r="17" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-    </row>
-    <row r="18" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-    </row>
-    <row r="19" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-    </row>
-    <row r="20" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-    </row>
-    <row r="30" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-    </row>
-    <row r="31" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-    </row>
-    <row r="32" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-    </row>
-    <row r="33" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-    </row>
-    <row r="34" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-    </row>
-    <row r="35" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="5"/>
-    </row>
-    <row r="36" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-    </row>
-    <row r="37" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-    </row>
-    <row r="38" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
-    </row>
-    <row r="39" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-    </row>
-    <row r="40" spans="6:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16"/>
+      <c r="I16" s="1"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17"/>
+      <c r="F17" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" s="4" customFormat="1" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20"/>
+      <c r="F20" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+    </row>
+    <row r="21" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21"/>
+      <c r="F21" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+    </row>
+    <row r="22" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22"/>
+      <c r="F22" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+    </row>
+    <row r="23" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23"/>
+      <c r="F23" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+    </row>
+    <row r="24" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24"/>
+      <c r="F24" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+    </row>
+    <row r="25" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25"/>
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+    </row>
+    <row r="26" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26"/>
+      <c r="F26" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+    </row>
+    <row r="27" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27"/>
+      <c r="F27" s="1">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+    </row>
+    <row r="28" spans="1:15" s="4" customFormat="1" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29"/>
+      <c r="F29" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="O29" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30"/>
+      <c r="F30" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="O30" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31"/>
+      <c r="F31" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="O31" s="1">
+        <v>0.44791666666666669</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32"/>
+      <c r="F32" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32" s="1">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="O32" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33"/>
+      <c r="F33" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0.51041666666666663</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" s="4" customFormat="1" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="3">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="O34" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="O35" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="O37" s="1">
+        <v>0.44791666666666669</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38" s="1">
+        <v>0.4375</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38" s="1">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="O38" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="O39" s="1">
+        <v>0.51041666666666663</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>15</v>
+      </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40" s="1">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="O40" s="1">
+        <v>0.54166666666666663</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -952,8 +1728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -2405,12 +3181,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004792E0B1DD728F47A9D3A151D94C43C2" ma:contentTypeVersion="2" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="8cbc72be1ef08462ba104cabf918da17">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6edaa03f-8cd3-4dde-a2dc-6fcdfb7e57e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6559be5467c1c92e09b21fd7a0e33ede" ns3:_="">
     <xsd:import namespace="6edaa03f-8cd3-4dde-a2dc-6fcdfb7e57e2"/>
@@ -2542,16 +3327,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD84CE38-E42E-4165-94C0-E9F0263CCA00}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85C72108-22AD-4B4C-AD2F-243F6F7C20B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -2567,7 +3351,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A788422-0B72-49B7-97E5-441D45C6B022}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2583,12 +3367,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD84CE38-E42E-4165-94C0-E9F0263CCA00}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>